<commit_message>
Allow not to press Enter when finish typing the name option in ketxuat
</commit_message>
<xml_diff>
--- a/My Excel File.xlsx
+++ b/My Excel File.xlsx
@@ -6,13 +6,14 @@
   <sheets>
     <sheet sheetId="1" name="nhap-thanhpham" state="visible" r:id="rId4"/>
     <sheet sheetId="2" name="xuat-thanhpham" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="ton-thanhpham" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
   <si>
     <t>Tên Hàng</t>
   </si>
@@ -499,4 +500,46 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="6" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>-100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix bug when edit name in nhap,xuat
</commit_message>
<xml_diff>
--- a/My Excel File.xlsx
+++ b/My Excel File.xlsx
@@ -4,56 +4,59 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="nhap-linhkien" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="xuat-linhkien" state="visible" r:id="rId5"/>
+    <sheet sheetId="1" name="nhap-thanhpham" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="xuat-thanhpham" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>Tên Hàng</t>
   </si>
   <si>
-    <t>Part Number</t>
+    <t>MCU</t>
   </si>
   <si>
     <t>Sổ Hợp Đồng</t>
   </si>
   <si>
-    <t>Sản Phẩm</t>
-  </si>
-  <si>
-    <t>Công Ty Nhập</t>
+    <t>Chip</t>
   </si>
   <si>
     <t>Ngày Nhập</t>
   </si>
   <si>
-    <t>Đơn Vị Tính</t>
-  </si>
-  <si>
     <t>Số Lượng</t>
   </si>
   <si>
-    <t>Đơn Giá</t>
-  </si>
-  <si>
-    <t>Thành Tiền</t>
-  </si>
-  <si>
-    <t>ha</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>2021-06-30</t>
-  </si>
-  <si>
-    <t>d</t>
+    <t>sản phẩm 2</t>
+  </si>
+  <si>
+    <t>11111111</t>
+  </si>
+  <si>
+    <t>111111</t>
+  </si>
+  <si>
+    <t>2021-07-08</t>
+  </si>
+  <si>
+    <t>sản phẩm 1</t>
+  </si>
+  <si>
+    <t>222222222</t>
+  </si>
+  <si>
+    <t>2222222</t>
+  </si>
+  <si>
+    <t>22222222222</t>
+  </si>
+  <si>
+    <t>2021-07-15</t>
   </si>
 </sst>
 </file>
@@ -430,13 +433,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:F3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,49 +458,45 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="H2">
-        <v>12</v>
-      </c>
-      <c r="I2">
-        <v>21</v>
-      </c>
-      <c r="J2">
-        <v>21</v>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -508,13 +507,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:F1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -532,18 +531,6 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bug when edit xuat: not allow to xuat the larger quantity than the storage has
</commit_message>
<xml_diff>
--- a/My Excel File.xlsx
+++ b/My Excel File.xlsx
@@ -4,59 +4,56 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="nhap-thanhpham" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="xuat-thanhpham" state="visible" r:id="rId5"/>
+    <sheet sheetId="1" name="nhap-linhkien" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="xuat-linhkien" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>Tên Hàng</t>
   </si>
   <si>
-    <t>MCU</t>
+    <t>Part Number</t>
   </si>
   <si>
     <t>Sổ Hợp Đồng</t>
   </si>
   <si>
-    <t>Chip</t>
+    <t>Sản Phẩm</t>
+  </si>
+  <si>
+    <t>Công Ty Nhập</t>
   </si>
   <si>
     <t>Ngày Nhập</t>
   </si>
   <si>
+    <t>Đơn Vị Tính</t>
+  </si>
+  <si>
     <t>Số Lượng</t>
   </si>
   <si>
-    <t>sản phẩm 2</t>
-  </si>
-  <si>
-    <t>11111111</t>
-  </si>
-  <si>
-    <t>111111</t>
-  </si>
-  <si>
-    <t>2021-07-08</t>
-  </si>
-  <si>
-    <t>sản phẩm 1</t>
-  </si>
-  <si>
-    <t>222222222</t>
-  </si>
-  <si>
-    <t>2222222</t>
-  </si>
-  <si>
-    <t>22222222222</t>
-  </si>
-  <si>
-    <t>2021-07-15</t>
+    <t>Đơn Giá</t>
+  </si>
+  <si>
+    <t>Thành Tiền</t>
+  </si>
+  <si>
+    <t>món hàng 1</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>2021-07-02</t>
+  </si>
+  <si>
+    <t>kg</t>
   </si>
 </sst>
 </file>
@@ -433,13 +430,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:J1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="6" width="20" customWidth="1"/>
+    <col min="1" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,45 +455,17 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="J1" t="s">
         <v>9</v>
-      </c>
-      <c r="F2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -507,13 +476,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:J2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="6" width="20" customWidth="1"/>
+    <col min="1" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -531,6 +500,50 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>1000</v>
+      </c>
+      <c r="I2">
+        <v>20</v>
+      </c>
+      <c r="J2">
+        <v>20000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bugs relating to ketxuat and name searches
</commit_message>
<xml_diff>
--- a/My Excel File.xlsx
+++ b/My Excel File.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Tên Hàng</t>
   </si>
@@ -44,16 +44,25 @@
     <t>Thành Tiền</t>
   </si>
   <si>
-    <t>món hàng 1</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>2021-07-02</t>
-  </si>
-  <si>
-    <t>kg</t>
+    <t>PCB -RF_SOC 2021.2.19( PHIÊN BẢN CŨ)</t>
+  </si>
+  <si>
+    <t>PCB RF SOC 1 PHA</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>MODULE RF 1P SOC</t>
+  </si>
+  <si>
+    <t>TỒN 30/06/2021</t>
+  </si>
+  <si>
+    <t>2021-06-30</t>
+  </si>
+  <si>
+    <t>Cái</t>
   </si>
 </sst>
 </file>
@@ -430,6 +439,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="10" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2">
+        <v>92</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
@@ -472,82 +559,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2">
-        <v>1000</v>
-      </c>
-      <c r="I2">
-        <v>20</v>
-      </c>
-      <c r="J2">
-        <v>20000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add message box when nhap, xuat, edit, search names, export file Excel
</commit_message>
<xml_diff>
--- a/My Excel File.xlsx
+++ b/My Excel File.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Tên Hàng</t>
   </si>
@@ -44,16 +44,16 @@
     <t>Thành Tiền</t>
   </si>
   <si>
-    <t>PCB -RF_SOC 2021.2.19( PHIÊN BẢN CŨ)</t>
-  </si>
-  <si>
-    <t>PCB RF SOC 1 PHA</t>
+    <t>PCB - RF_1pha_HT32F5_Si4432_E19_E49_ESRF_V1.3- 03022021 Size 45x65mm</t>
+  </si>
+  <si>
+    <t>LF_1pha_HT32F5 V1.3_03022021</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>MODULE RF 1P SOC</t>
+    <t>MODULE RF 1P HOLTEK</t>
   </si>
   <si>
     <t>TỒN 30/06/2021</t>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>Cái</t>
+  </si>
+  <si>
+    <t>MODULE RF 1P HOTEK</t>
+  </si>
+  <si>
+    <t>CTY TNHH YEAR2000</t>
+  </si>
+  <si>
+    <t>2021-07-01</t>
   </si>
 </sst>
 </file>
@@ -500,7 +509,7 @@
         <v>16</v>
       </c>
       <c r="H2">
-        <v>92</v>
+        <v>266704</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -517,7 +526,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="10" width="20" customWidth="1"/>
@@ -555,6 +564,38 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
New Update: Autocomplete input
</commit_message>
<xml_diff>
--- a/My Excel File.xlsx
+++ b/My Excel File.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Tên Hàng</t>
   </si>
@@ -44,16 +44,16 @@
     <t>Thành Tiền</t>
   </si>
   <si>
-    <t>PCB - RF_1pha_HT32F5_Si4432_E19_E49_ESRF_V1.3- 03022021 Size 45x65mm</t>
-  </si>
-  <si>
-    <t>LF_1pha_HT32F5 V1.3_03022021</t>
+    <t>DCU_2G(Sim800C)_4G(Sim7600CE)_SF80P20_Cover_1603757518</t>
+  </si>
+  <si>
+    <t>DCU-NEW-V4.2-231020</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>MODULE RF 1P HOLTEK</t>
+    <t>DCU RF 2G</t>
   </si>
   <si>
     <t>TỒN 30/06/2021</t>
@@ -63,15 +63,6 @@
   </si>
   <si>
     <t>Cái</t>
-  </si>
-  <si>
-    <t>MODULE RF 1P HOTEK</t>
-  </si>
-  <si>
-    <t>CTY TNHH YEAR2000</t>
-  </si>
-  <si>
-    <t>2021-07-01</t>
   </si>
 </sst>
 </file>
@@ -509,7 +500,7 @@
         <v>16</v>
       </c>
       <c r="H2">
-        <v>266704</v>
+        <v>49</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -526,7 +517,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="10" width="20" customWidth="1"/>
@@ -564,38 +555,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2">
-        <v>100</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Super Update: Save keywords via firestore; Add excel keywords; allow ketxuat ton; can see log-nhap, log-xuat in cslk, cstp pages
</commit_message>
<xml_diff>
--- a/My Excel File.xlsx
+++ b/My Excel File.xlsx
@@ -6,13 +6,14 @@
   <sheets>
     <sheet sheetId="1" name="nhap-linhkien" state="visible" r:id="rId4"/>
     <sheet sheetId="2" name="xuat-linhkien" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="ton-linhkien" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
   <si>
     <t>Tên Hàng</t>
   </si>
@@ -63,6 +64,57 @@
   </si>
   <si>
     <t>Cái</t>
+  </si>
+  <si>
+    <t>PCB RF 1 PHA STM8S005-Si4432</t>
+  </si>
+  <si>
+    <t>MODULE RF 1P STM8</t>
+  </si>
+  <si>
+    <t>PCB -RF_SOC 2021.2.19( PHIÊN BẢN CŨ)</t>
+  </si>
+  <si>
+    <t>PCB RF SOC 1 PHA</t>
+  </si>
+  <si>
+    <t>MODULE RF 1P SOC</t>
+  </si>
+  <si>
+    <t>PCB - RF_1pha_HT32F5_Si4432_E19_E49_ESRF_V1.3- 03022021 Size 45x65mm</t>
+  </si>
+  <si>
+    <t>LF_1pha_HT32F5 V1.3_03022021</t>
+  </si>
+  <si>
+    <t>MODULE RF 1P HOLTEK</t>
+  </si>
+  <si>
+    <t>Danh</t>
+  </si>
+  <si>
+    <t>Ceramic Cap 0402 270p 50V 5% NP0</t>
+  </si>
+  <si>
+    <t>hopdong01</t>
+  </si>
+  <si>
+    <t>sanpham01</t>
+  </si>
+  <si>
+    <t>cty01</t>
+  </si>
+  <si>
+    <t>2021-07-15</t>
+  </si>
+  <si>
+    <t>MODULE RF 1P HOTEK</t>
+  </si>
+  <si>
+    <t>CTY TNHH YEAR2000</t>
+  </si>
+  <si>
+    <t>2021-07-01</t>
   </si>
 </sst>
 </file>
@@ -439,6 +491,212 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J6"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="10" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2">
+        <v>49</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3">
+        <v>17200</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>92</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5">
+        <v>266704</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
@@ -479,28 +737,28 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
         <v>16</v>
       </c>
       <c r="H2">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -515,44 +773,67 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:C5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>266604</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New feature: in ketxuat page, we can preview what is inside the Excel file without opening it
</commit_message>
<xml_diff>
--- a/My Excel File.xlsx
+++ b/My Excel File.xlsx
@@ -6,13 +6,14 @@
   <sheets>
     <sheet sheetId="1" name="nhap-linhkien" state="visible" r:id="rId4"/>
     <sheet sheetId="2" name="xuat-linhkien" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="ton-linhkien" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
   <si>
     <t>Tên Hàng</t>
   </si>
@@ -44,13 +45,73 @@
     <t>Thành Tiền</t>
   </si>
   <si>
+    <t>DCU_2G(Sim800C)_4G(Sim7600CE)_SF80P20_Cover_1603757518</t>
+  </si>
+  <si>
+    <t>DCU-NEW-V4.2-231020</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>DCU RF 2G</t>
+  </si>
+  <si>
+    <t>TỒN 30/06/2021</t>
+  </si>
+  <si>
+    <t>2021-06-30</t>
+  </si>
+  <si>
+    <t>Cái</t>
+  </si>
+  <si>
+    <t>danh</t>
+  </si>
+  <si>
+    <t>PCB RF 1 PHA STM8S005-Si4432</t>
+  </si>
+  <si>
+    <t>MODULE RF 1P STM8</t>
+  </si>
+  <si>
+    <t>PCB -RF_SOC 2021.2.19( PHIÊN BẢN CŨ)</t>
+  </si>
+  <si>
+    <t>PCB RF SOC 1 PHA</t>
+  </si>
+  <si>
+    <t>MODULE RF 1P SOC</t>
+  </si>
+  <si>
     <t>PCB - RF_1pha_HT32F5_Si4432_E19_E49_ESRF_V1.3- 03022021 Size 45x65mm</t>
   </si>
   <si>
     <t>LF_1pha_HT32F5 V1.3_03022021</t>
   </si>
   <si>
-    <t/>
+    <t>MODULE RF 1P HOLTEK</t>
+  </si>
+  <si>
+    <t>Ceramic Cap 0402 270p 50V 5% NP0</t>
+  </si>
+  <si>
+    <t>GRM1555C1H271JA01D</t>
+  </si>
+  <si>
+    <t>sohopdong01</t>
+  </si>
+  <si>
+    <t>sanpham02</t>
+  </si>
+  <si>
+    <t>cty01</t>
+  </si>
+  <si>
+    <t>2021-08-01</t>
+  </si>
+  <si>
+    <t>cái</t>
   </si>
   <si>
     <t>MODULE RF 1P HOTEK</t>
@@ -60,9 +121,6 @@
   </si>
   <si>
     <t>2021-07-01</t>
-  </si>
-  <si>
-    <t>Cái</t>
   </si>
 </sst>
 </file>
@@ -439,7 +497,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="10" width="20" customWidth="1"/>
@@ -475,6 +533,166 @@
       </c>
       <c r="J1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2">
+        <v>49</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3">
+        <v>17200</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>92</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5">
+        <v>266704</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <v>21</v>
+      </c>
+      <c r="J6">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -525,22 +743,22 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
         <v>16</v>
@@ -553,6 +771,97 @@
       </c>
       <c r="J2">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="3" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>-17200</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>266604</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>17200</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switch positions between tenhang and partnum in the excel file
</commit_message>
<xml_diff>
--- a/My Excel File.xlsx
+++ b/My Excel File.xlsx
@@ -13,14 +13,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+  <si>
+    <t>Part Number</t>
+  </si>
   <si>
     <t>Tên Hàng</t>
   </si>
   <si>
-    <t>Part Number</t>
-  </si>
-  <si>
     <t>Sổ Hợp Đồng</t>
   </si>
   <si>
@@ -45,12 +45,12 @@
     <t>Thành Tiền</t>
   </si>
   <si>
+    <t>DCU-NEW-V4.2-231020</t>
+  </si>
+  <si>
     <t>DCU_2G(Sim800C)_4G(Sim7600CE)_SF80P20_Cover_1603757518</t>
   </si>
   <si>
-    <t>DCU-NEW-V4.2-231020</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -66,37 +66,28 @@
     <t>Cái</t>
   </si>
   <si>
-    <t>danh</t>
-  </si>
-  <si>
-    <t>PCB RF 1 PHA STM8S005-Si4432</t>
-  </si>
-  <si>
-    <t>MODULE RF 1P STM8</t>
+    <t>PCB RF SOC 1 PHA</t>
   </si>
   <si>
     <t>PCB -RF_SOC 2021.2.19( PHIÊN BẢN CŨ)</t>
   </si>
   <si>
-    <t>PCB RF SOC 1 PHA</t>
-  </si>
-  <si>
     <t>MODULE RF 1P SOC</t>
   </si>
   <si>
+    <t>LF_1pha_HT32F5 V1.3_03022021</t>
+  </si>
+  <si>
     <t>PCB - RF_1pha_HT32F5_Si4432_E19_E49_ESRF_V1.3- 03022021 Size 45x65mm</t>
   </si>
   <si>
-    <t>LF_1pha_HT32F5 V1.3_03022021</t>
-  </si>
-  <si>
     <t>MODULE RF 1P HOLTEK</t>
   </si>
   <si>
+    <t>GRM1555C1H271JA01D</t>
+  </si>
+  <si>
     <t>Ceramic Cap 0402 270p 50V 5% NP0</t>
-  </si>
-  <si>
-    <t>GRM1555C1H271JA01D</t>
   </si>
   <si>
     <t>sohopdong01</t>
@@ -497,7 +488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="10" width="20" customWidth="1"/>
@@ -590,7 +581,7 @@
         <v>16</v>
       </c>
       <c r="H3">
-        <v>17200</v>
+        <v>92</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -622,7 +613,7 @@
         <v>16</v>
       </c>
       <c r="H4">
-        <v>92</v>
+        <v>266704</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -639,59 +630,27 @@
         <v>24</v>
       </c>
       <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5">
-        <v>266704</v>
-      </c>
       <c r="I5">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6">
-        <v>12</v>
-      </c>
-      <c r="I6">
-        <v>21</v>
-      </c>
-      <c r="J6">
         <v>252</v>
       </c>
     </row>
@@ -743,22 +702,22 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G2" t="s">
         <v>16</v>
@@ -781,7 +740,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="20" customWidth="1"/>
@@ -789,7 +748,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -800,7 +759,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>92</v>
@@ -811,10 +770,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B3">
-        <v>-17200</v>
+        <v>266604</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
@@ -822,10 +781,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>266604</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -833,35 +792,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B5">
-        <v>17200</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>49</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New feature: Save submission date to database
</commit_message>
<xml_diff>
--- a/My Excel File.xlsx
+++ b/My Excel File.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
   <si>
     <t>Part Number</t>
   </si>
@@ -43,75 +43,6 @@
   </si>
   <si>
     <t>Thành Tiền</t>
-  </si>
-  <si>
-    <t>DCU-NEW-V4.2-231020</t>
-  </si>
-  <si>
-    <t>DCU_2G(Sim800C)_4G(Sim7600CE)_SF80P20_Cover_1603757518</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>DCU RF 2G</t>
-  </si>
-  <si>
-    <t>TỒN 30/06/2021</t>
-  </si>
-  <si>
-    <t>2021-06-30</t>
-  </si>
-  <si>
-    <t>Cái</t>
-  </si>
-  <si>
-    <t>PCB RF SOC 1 PHA</t>
-  </si>
-  <si>
-    <t>PCB -RF_SOC 2021.2.19( PHIÊN BẢN CŨ)</t>
-  </si>
-  <si>
-    <t>MODULE RF 1P SOC</t>
-  </si>
-  <si>
-    <t>LF_1pha_HT32F5 V1.3_03022021</t>
-  </si>
-  <si>
-    <t>PCB - RF_1pha_HT32F5_Si4432_E19_E49_ESRF_V1.3- 03022021 Size 45x65mm</t>
-  </si>
-  <si>
-    <t>MODULE RF 1P HOLTEK</t>
-  </si>
-  <si>
-    <t>GRM1555C1H271JA01D</t>
-  </si>
-  <si>
-    <t>Ceramic Cap 0402 270p 50V 5% NP0</t>
-  </si>
-  <si>
-    <t>sohopdong01</t>
-  </si>
-  <si>
-    <t>sanpham02</t>
-  </si>
-  <si>
-    <t>cty01</t>
-  </si>
-  <si>
-    <t>2021-08-01</t>
-  </si>
-  <si>
-    <t>cái</t>
-  </si>
-  <si>
-    <t>MODULE RF 1P HOTEK</t>
-  </si>
-  <si>
-    <t>CTY TNHH YEAR2000</t>
-  </si>
-  <si>
-    <t>2021-07-01</t>
   </si>
 </sst>
 </file>
@@ -488,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="10" width="20" customWidth="1"/>
@@ -526,134 +457,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2">
-        <v>49</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3">
-        <v>92</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4">
-        <v>266704</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5">
-        <v>12</v>
-      </c>
-      <c r="I5">
-        <v>21</v>
-      </c>
-      <c r="J5">
-        <v>252</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -662,7 +465,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="10" width="20" customWidth="1"/>
@@ -700,38 +503,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2">
-        <v>100</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -740,7 +511,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="20" customWidth="1"/>
@@ -757,50 +528,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2">
-        <v>92</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3">
-        <v>266604</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>49</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Brand new feature: allow searching documentsvia sohopdong in chinhsua, ketxuat pages
</commit_message>
<xml_diff>
--- a/My Excel File.xlsx
+++ b/My Excel File.xlsx
@@ -4,45 +4,47 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="nhap-linhkien" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="xuat-linhkien" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="ton-linhkien" state="visible" r:id="rId6"/>
+    <sheet sheetId="1" name="nhap-thanhpham" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="xuat-thanhpham" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
-  <si>
-    <t>Part Number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Tên Hàng</t>
   </si>
   <si>
+    <t>MCU</t>
+  </si>
+  <si>
     <t>Sổ Hợp Đồng</t>
   </si>
   <si>
-    <t>Sản Phẩm</t>
-  </si>
-  <si>
-    <t>Công Ty Nhập</t>
+    <t>Chip</t>
   </si>
   <si>
     <t>Ngày Nhập</t>
   </si>
   <si>
-    <t>Đơn Vị Tính</t>
-  </si>
-  <si>
     <t>Số Lượng</t>
   </si>
   <si>
-    <t>Đơn Giá</t>
-  </si>
-  <si>
-    <t>Thành Tiền</t>
+    <t>LED Green</t>
+  </si>
+  <si>
+    <t>mcu01</t>
+  </si>
+  <si>
+    <t>sohopdong01</t>
+  </si>
+  <si>
+    <t>chip01</t>
+  </si>
+  <si>
+    <t>2021-09-02</t>
   </si>
 </sst>
 </file>
@@ -419,13 +421,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:F2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,17 +446,25 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="D2" t="s">
         <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -465,13 +475,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:F1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,43 +499,6 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="3" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New feature: Delete reviews
</commit_message>
<xml_diff>
--- a/My Excel File.xlsx
+++ b/My Excel File.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Part Number</t>
   </si>
@@ -43,6 +43,27 @@
   </si>
   <si>
     <t>Thành Tiền</t>
+  </si>
+  <si>
+    <t>GRM219R61A106KE44D</t>
+  </si>
+  <si>
+    <t>Ceramic Cap 0805 10uF 10V 10% X5R</t>
+  </si>
+  <si>
+    <t>sohopdong01</t>
+  </si>
+  <si>
+    <t>sanpham01</t>
+  </si>
+  <si>
+    <t>cty01</t>
+  </si>
+  <si>
+    <t>2021-09-11</t>
+  </si>
+  <si>
+    <t>Cái</t>
   </si>
 </sst>
 </file>
@@ -419,7 +440,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="10" width="20" customWidth="1"/>
@@ -455,6 +476,38 @@
       </c>
       <c r="J1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2">
+        <v>12</v>
+      </c>
+      <c r="I2">
+        <v>21</v>
+      </c>
+      <c r="J2">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -511,7 +564,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="20" customWidth="1"/>
@@ -528,6 +581,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
Change a little bit
</commit_message>
<xml_diff>
--- a/My Excel File.xlsx
+++ b/My Excel File.xlsx
@@ -4,66 +4,50 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="nhap-linhkien" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="xuat-linhkien" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="ton-linhkien" state="visible" r:id="rId6"/>
+    <sheet sheetId="1" name="nhap-thanhpham" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="xuat-thanhpham" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
-  <si>
-    <t>Part Number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Tên Hàng</t>
   </si>
   <si>
+    <t>MCU</t>
+  </si>
+  <si>
     <t>Sổ Hợp Đồng</t>
   </si>
   <si>
-    <t>Sản Phẩm</t>
-  </si>
-  <si>
-    <t>Công Ty Nhập</t>
+    <t>Chip</t>
   </si>
   <si>
     <t>Ngày Nhập</t>
   </si>
   <si>
-    <t>Đơn Vị Tính</t>
-  </si>
-  <si>
     <t>Số Lượng</t>
   </si>
   <si>
-    <t>Đơn Giá</t>
-  </si>
-  <si>
-    <t>Thành Tiền</t>
-  </si>
-  <si>
-    <t>GRM219R61A106KE44D</t>
-  </si>
-  <si>
-    <t>Ceramic Cap 0805 10uF 10V 10% X5R</t>
-  </si>
-  <si>
-    <t>sohopdong01</t>
-  </si>
-  <si>
-    <t>sanpham01</t>
-  </si>
-  <si>
-    <t>cty01</t>
-  </si>
-  <si>
-    <t>2021-09-11</t>
-  </si>
-  <si>
-    <t>Cái</t>
+    <t>danh</t>
+  </si>
+  <si>
+    <t>mcu01</t>
+  </si>
+  <si>
+    <t>16/2021/DT-FE - 03/06/2021</t>
+  </si>
+  <si>
+    <t>chip01</t>
+  </si>
+  <si>
+    <t>2021-09-26</t>
+  </si>
+  <si>
+    <t>sinh</t>
   </si>
 </sst>
 </file>
@@ -440,13 +424,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:F3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,49 +449,45 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2">
-        <v>12</v>
-      </c>
-      <c r="I2">
-        <v>21</v>
-      </c>
-      <c r="J2">
-        <v>252</v>
+      <c r="F3">
+        <v>1200</v>
       </c>
     </row>
   </sheetData>
@@ -518,13 +498,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:F1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,54 +522,6 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="3" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit documents via grid
</commit_message>
<xml_diff>
--- a/My Excel File.xlsx
+++ b/My Excel File.xlsx
@@ -4,71 +4,57 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="nhap-linhkien" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="xuat-linhkien" state="visible" r:id="rId5"/>
+    <sheet sheetId="1" name="nhap-thanhpham" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="xuat-thanhpham" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="ton-thanhpham" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
-  <si>
-    <t>Part Number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>Tên Hàng</t>
   </si>
   <si>
+    <t>MCU</t>
+  </si>
+  <si>
     <t>Sổ Hợp Đồng</t>
   </si>
   <si>
-    <t>Sản Phẩm</t>
-  </si>
-  <si>
-    <t>Công Ty Nhập</t>
+    <t>Chip</t>
   </si>
   <si>
     <t>Ngày Nhập</t>
   </si>
   <si>
+    <t>Số Lượng</t>
+  </si>
+  <si>
+    <t>smooth</t>
+  </si>
+  <si>
+    <t>mcu</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>chip</t>
+  </si>
+  <si>
+    <t>2021-10-05</t>
+  </si>
+  <si>
+    <t>2021-10-06</t>
+  </si>
+  <si>
     <t>Đơn Vị Tính</t>
   </si>
   <si>
-    <t>Số Lượng</t>
-  </si>
-  <si>
-    <t>Đơn Giá</t>
-  </si>
-  <si>
-    <t>Thành Tiền</t>
-  </si>
-  <si>
-    <t>LB1117AATB-3.3</t>
-  </si>
-  <si>
-    <t>1A LOW DROPOUT LINEAR REGULATOR</t>
-  </si>
-  <si>
-    <t>5445</t>
-  </si>
-  <si>
-    <t>fds</t>
-  </si>
-  <si>
-    <t>edsrf</t>
-  </si>
-  <si>
-    <t>4654-06-05</t>
-  </si>
-  <si>
-    <t>cai</t>
-  </si>
-  <si>
-    <t>543654.0000</t>
-  </si>
-  <si>
-    <t>234858528.0000</t>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -445,13 +431,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:F2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,49 +456,25 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2">
-        <v>432</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
+      <c r="F2">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -523,13 +485,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:F2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -548,17 +510,61 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="D2" t="s">
         <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="3" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V1.5: check internet connection status
</commit_message>
<xml_diff>
--- a/My Excel File.xlsx
+++ b/My Excel File.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>Part Number</t>
   </si>
@@ -45,85 +45,52 @@
     <t>Thành Tiền</t>
   </si>
   <si>
-    <t>tinh</t>
-  </si>
-  <si>
-    <t>yeu</t>
-  </si>
-  <si>
-    <t>da</t>
-  </si>
-  <si>
-    <t>phai</t>
-  </si>
-  <si>
-    <t>mo</t>
-  </si>
-  <si>
-    <t>2021-10-06</t>
+    <t>GRM1555C1H271JA01D</t>
+  </si>
+  <si>
+    <t>Ceramic Cap 0402 270p 50V 5% NP0</t>
+  </si>
+  <si>
+    <t>sohopdong01</t>
+  </si>
+  <si>
+    <t>sanpham01</t>
+  </si>
+  <si>
+    <t>cty01</t>
+  </si>
+  <si>
+    <t>2021-10-10</t>
   </si>
   <si>
     <t>cái</t>
   </si>
   <si>
-    <t>2.0000</t>
-  </si>
-  <si>
-    <t>4444.0000</t>
-  </si>
-  <si>
-    <t>em</t>
-  </si>
-  <si>
-    <t>ra</t>
-  </si>
-  <si>
-    <t>4.0000</t>
-  </si>
-  <si>
-    <t>mùa</t>
-  </si>
-  <si>
-    <t>thu</t>
-  </si>
-  <si>
-    <t>mang</t>
-  </si>
-  <si>
-    <t>nho</t>
-  </si>
-  <si>
-    <t>anh</t>
-  </si>
-  <si>
-    <t>km</t>
-  </si>
-  <si>
-    <t>GJM1555C1H2R7CB01D</t>
-  </si>
-  <si>
-    <t>Ceramic Cap 0402 2.7pF 50V +-0.25p NP0</t>
-  </si>
-  <si>
-    <t>sohopdong01</t>
-  </si>
-  <si>
-    <t>sanpham01</t>
-  </si>
-  <si>
-    <t>cty01</t>
-  </si>
-  <si>
-    <t>2021-10-09</t>
-  </si>
-  <si>
-    <t>21.0000</t>
+    <t>21.00</t>
   </si>
   <si>
     <t>252.0000</t>
   </si>
   <si>
-    <t>198.0000</t>
+    <t>S1M-13-F</t>
+  </si>
+  <si>
+    <t>S1M</t>
+  </si>
+  <si>
+    <t>sohopdong02</t>
+  </si>
+  <si>
+    <t>sanpham02</t>
+  </si>
+  <si>
+    <t>cty02</t>
+  </si>
+  <si>
+    <t>10.69</t>
+  </si>
+  <si>
+    <t>235.1800</t>
   </si>
 </sst>
 </file>
@@ -500,7 +467,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="10" width="20" customWidth="1"/>
@@ -561,7 +528,7 @@
         <v>16</v>
       </c>
       <c r="H2">
-        <v>2222</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s">
         <v>17</v>
@@ -575,16 +542,16 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
@@ -593,109 +560,13 @@
         <v>16</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5">
-        <v>12</v>
-      </c>
-      <c r="I5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6">
-        <v>12</v>
-      </c>
-      <c r="I6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -706,7 +577,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="10" width="20" customWidth="1"/>
@@ -742,38 +613,6 @@
       </c>
       <c r="J1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2">
-        <v>99</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -784,7 +623,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="20" customWidth="1"/>
@@ -803,10 +642,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -814,34 +653,12 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>2123</v>
-      </c>
-      <c r="C5" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v1.0.6: bug fixes and new feature: save last submission
</commit_message>
<xml_diff>
--- a/My Excel File.xlsx
+++ b/My Excel File.xlsx
@@ -4,93 +4,36 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="nhap-linhkien" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="xuat-linhkien" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="ton-linhkien" state="visible" r:id="rId6"/>
+    <sheet sheetId="1" name="nhap-thanhpham" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="xuat-thanhpham" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="ton-thanhpham" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
-  <si>
-    <t>Part Number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>Tên Hàng</t>
   </si>
   <si>
+    <t>MCU</t>
+  </si>
+  <si>
     <t>Sổ Hợp Đồng</t>
   </si>
   <si>
-    <t>Sản Phẩm</t>
-  </si>
-  <si>
-    <t>Công Ty Nhập</t>
+    <t>Chip</t>
   </si>
   <si>
     <t>Ngày Nhập</t>
   </si>
   <si>
+    <t>Số Lượng</t>
+  </si>
+  <si>
     <t>Đơn Vị Tính</t>
-  </si>
-  <si>
-    <t>Số Lượng</t>
-  </si>
-  <si>
-    <t>Đơn Giá</t>
-  </si>
-  <si>
-    <t>Thành Tiền</t>
-  </si>
-  <si>
-    <t>GRM1555C1H271JA01D</t>
-  </si>
-  <si>
-    <t>Ceramic Cap 0402 270p 50V 5% NP0</t>
-  </si>
-  <si>
-    <t>sohopdong01</t>
-  </si>
-  <si>
-    <t>sanpham01</t>
-  </si>
-  <si>
-    <t>cty01</t>
-  </si>
-  <si>
-    <t>2021-10-10</t>
-  </si>
-  <si>
-    <t>cái</t>
-  </si>
-  <si>
-    <t>21.00</t>
-  </si>
-  <si>
-    <t>252.0000</t>
-  </si>
-  <si>
-    <t>S1M-13-F</t>
-  </si>
-  <si>
-    <t>S1M</t>
-  </si>
-  <si>
-    <t>sohopdong02</t>
-  </si>
-  <si>
-    <t>sanpham02</t>
-  </si>
-  <si>
-    <t>cty02</t>
-  </si>
-  <si>
-    <t>10.69</t>
-  </si>
-  <si>
-    <t>235.1800</t>
   </si>
 </sst>
 </file>
@@ -467,13 +410,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:F1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,82 +434,6 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -577,13 +444,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:F1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -601,18 +468,6 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -623,7 +478,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="20" customWidth="1"/>
@@ -631,35 +486,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.0.9: fix minor bugs
</commit_message>
<xml_diff>
--- a/My Excel File.xlsx
+++ b/My Excel File.xlsx
@@ -4,60 +4,45 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="nhap-thanhpham" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="xuat-thanhpham" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="ton-thanhpham" state="visible" r:id="rId6"/>
+    <sheet sheetId="1" name="nhap-linhkien" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="xuat-linhkien" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="ton-linhkien" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
+  <si>
+    <t>Part Number</t>
+  </si>
   <si>
     <t>Tên Hàng</t>
   </si>
   <si>
-    <t>MCU</t>
-  </si>
-  <si>
     <t>Sổ Hợp Đồng</t>
   </si>
   <si>
-    <t>Chip</t>
+    <t>Sản Phẩm</t>
+  </si>
+  <si>
+    <t>Công Ty Nhập</t>
   </si>
   <si>
     <t>Ngày Nhập</t>
   </si>
   <si>
+    <t>Đơn Vị Tính</t>
+  </si>
+  <si>
     <t>Số Lượng</t>
   </si>
   <si>
-    <t>RES 0R 5% 3/4W 2010</t>
-  </si>
-  <si>
-    <t>mcu01</t>
-  </si>
-  <si>
-    <t>006-21/DT-BS</t>
-  </si>
-  <si>
-    <t>chip01</t>
-  </si>
-  <si>
-    <t>2021-10-11</t>
-  </si>
-  <si>
-    <t>Part Number</t>
-  </si>
-  <si>
-    <t>Đơn Vị Tính</t>
-  </si>
-  <si>
-    <t>AC2010JK-070RL</t>
-  </si>
-  <si>
-    <t>none</t>
+    <t>Đơn Giá</t>
+  </si>
+  <si>
+    <t>Thành Tiền</t>
   </si>
 </sst>
 </file>
@@ -434,13 +419,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:J1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="6" width="20" customWidth="1"/>
+    <col min="1" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,25 +444,17 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="J1" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -488,13 +465,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:J1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="6" width="20" customWidth="1"/>
+    <col min="1" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,6 +489,18 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -522,7 +511,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="20" customWidth="1"/>
@@ -530,24 +519,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.1.0: fix minor bugs and display totalThanhtien after exporting to Excel
</commit_message>
<xml_diff>
--- a/My Excel File.xlsx
+++ b/My Excel File.xlsx
@@ -4,45 +4,54 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="nhap-linhkien" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="xuat-linhkien" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="ton-linhkien" state="visible" r:id="rId6"/>
+    <sheet sheetId="1" name="nhap-thanhpham" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="xuat-thanhpham" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="ton-thanhpham" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
-  <si>
-    <t>Part Number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>Tên Hàng</t>
   </si>
   <si>
+    <t>MCU</t>
+  </si>
+  <si>
     <t>Sổ Hợp Đồng</t>
   </si>
   <si>
-    <t>Sản Phẩm</t>
-  </si>
-  <si>
-    <t>Công Ty Nhập</t>
+    <t>Chip</t>
   </si>
   <si>
     <t>Ngày Nhập</t>
   </si>
   <si>
+    <t>Số Lượng</t>
+  </si>
+  <si>
+    <t>RES 0R 5% 3/4W 2010</t>
+  </si>
+  <si>
+    <t>mcu01</t>
+  </si>
+  <si>
+    <t>006-21/DT-BS</t>
+  </si>
+  <si>
+    <t>chip01</t>
+  </si>
+  <si>
+    <t>2021-10-11</t>
+  </si>
+  <si>
     <t>Đơn Vị Tính</t>
   </si>
   <si>
-    <t>Số Lượng</t>
-  </si>
-  <si>
-    <t>Đơn Giá</t>
-  </si>
-  <si>
-    <t>Thành Tiền</t>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -419,13 +428,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:F2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,17 +453,25 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="D2" t="s">
         <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -465,13 +482,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:F1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,18 +506,6 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -511,7 +516,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="20" customWidth="1"/>
@@ -522,10 +527,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>